<commit_message>
sofia | fore peak tank curve | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Tank_curve.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Tank_curve.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97376A47-91EB-495A-B8C8-7BB99F99B77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B623CD3-3F4F-4D77-B843-D9A5164B98AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="887" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Трюм 1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="24">
   <si>
     <t>H</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>6838.74^</t>
-  </si>
-  <si>
-    <t>0 394</t>
   </si>
   <si>
     <t>-0 027</t>
@@ -596,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O83" sqref="N81:O83"/>
     </sheetView>
   </sheetViews>
@@ -3548,7 +3545,7 @@
         <v>-5.5220000000000002</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="4">
         <v>95.417000000000002</v>
@@ -3663,7 +3660,7 @@
         <v>-5.7240000000000002</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="4">
         <v>145.95599999999999</v>
@@ -11540,7 +11537,7 @@
         <v>-7.2629999999999999</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F88" s="4">
         <v>0</v>
@@ -14456,7 +14453,7 @@
         <v>1.3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2">
         <v>87.650999999999996</v>
@@ -14548,7 +14545,7 @@
         <v>1.7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2">
         <v>87.712000000000003</v>
@@ -23408,7 +23405,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B48" s="2">
         <v>72</v>
@@ -25999,7 +25996,7 @@
         <v>2.1459999999999999</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2">
         <v>7.3010000000000002</v>
@@ -36598,7 +36595,7 @@
         <v>5.0039999999999996</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F39" s="4">
         <v>14.343999999999999</v>
@@ -38718,7 +38715,7 @@
         <v>-4.8579999999999997</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F33" s="4">
         <v>0</v>
@@ -40882,9 +40879,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:G66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41094,8 +41091,8 @@
       <c r="D9" s="2">
         <v>1E-3</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
+      <c r="E9" s="2">
+        <v>0.39400000000000002</v>
       </c>
       <c r="F9" s="4">
         <v>41.252000000000002</v>
@@ -41989,7 +41986,7 @@
         <v>121.934</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E48" s="2">
         <v>2.35</v>
@@ -42006,7 +42003,7 @@
         <v>4.7</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C49" s="2">
         <v>121.93300000000001</v>
@@ -42127,7 +42124,7 @@
         <v>121.92400000000001</v>
       </c>
       <c r="D54" s="2">
-        <v>-33</v>
+        <v>-3.3000000000000002E-2</v>
       </c>
       <c r="E54" s="2">
         <v>2.669</v>
@@ -48867,7 +48864,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="4">
         <v>1037.579</v>
@@ -52446,7 +52443,7 @@
         <v>-2.6059999999999999</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="4">
         <v>251.023</v>
@@ -52492,7 +52489,7 @@
         <v>-2.698</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="4">
         <v>278.59899999999999</v>

</xml_diff>

<commit_message>
sofia | tank 211 curve | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Tank_curve.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Tank_curve.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B623CD3-3F4F-4D77-B843-D9A5164B98AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C65C28-AA6D-4ED7-A2DB-0777F3699E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="887" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="887" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Трюм 1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="22">
   <si>
     <t>H</t>
   </si>
@@ -107,12 +107,6 @@
   </si>
   <si>
     <t>0 050</t>
-  </si>
-  <si>
-    <t>0 320</t>
-  </si>
-  <si>
-    <t>0 428</t>
   </si>
   <si>
     <t>0 051</t>
@@ -3545,7 +3539,7 @@
         <v>-5.5220000000000002</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" s="4">
         <v>95.417000000000002</v>
@@ -3660,7 +3654,7 @@
         <v>-5.7240000000000002</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8" s="4">
         <v>145.95599999999999</v>
@@ -11537,7 +11531,7 @@
         <v>-7.2629999999999999</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F88" s="4">
         <v>0</v>
@@ -14453,7 +14447,7 @@
         <v>1.3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2">
         <v>87.650999999999996</v>
@@ -14545,7 +14539,7 @@
         <v>1.7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2">
         <v>87.712000000000003</v>
@@ -23405,7 +23399,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B48" s="2">
         <v>72</v>
@@ -25996,7 +25990,7 @@
         <v>2.1459999999999999</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2">
         <v>7.3010000000000002</v>
@@ -36595,7 +36589,7 @@
         <v>5.0039999999999996</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F39" s="4">
         <v>14.343999999999999</v>
@@ -38715,7 +38709,7 @@
         <v>-4.8579999999999997</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F33" s="4">
         <v>0</v>
@@ -40879,9 +40873,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52254,8 +52248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52304,7 +52298,7 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="4">
         <v>0</v>
       </c>
       <c r="F2" s="4">
@@ -52327,8 +52321,8 @@
       <c r="D3" s="2">
         <v>-2.1749999999999998</v>
       </c>
-      <c r="E3" s="2">
-        <v>53</v>
+      <c r="E3" s="4">
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="F3" s="4">
         <v>146.655</v>
@@ -52350,7 +52344,7 @@
       <c r="D4" s="2">
         <v>-2.3170000000000002</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <v>0.106</v>
       </c>
       <c r="F4" s="4">
@@ -52373,7 +52367,7 @@
       <c r="D5" s="2">
         <v>-2.4129999999999998</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>0.159</v>
       </c>
       <c r="F5" s="4">
@@ -52396,7 +52390,7 @@
       <c r="D6" s="2">
         <v>-2.488</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="4">
         <v>0.21299999999999999</v>
       </c>
       <c r="F6" s="4">
@@ -52419,7 +52413,7 @@
       <c r="D7" s="2">
         <v>-2.5510000000000002</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>0.26600000000000001</v>
       </c>
       <c r="F7" s="4">
@@ -52442,8 +52436,8 @@
       <c r="D8" s="2">
         <v>-2.6059999999999999</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
+      <c r="E8" s="4">
+        <v>0.32</v>
       </c>
       <c r="F8" s="4">
         <v>251.023</v>
@@ -52465,7 +52459,7 @@
       <c r="D9" s="2">
         <v>-2.6539999999999999</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="4">
         <v>0.374</v>
       </c>
       <c r="F9" s="4">
@@ -52488,8 +52482,8 @@
       <c r="D10" s="2">
         <v>-2.698</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>14</v>
+      <c r="E10" s="4">
+        <v>0.42799999999999999</v>
       </c>
       <c r="F10" s="4">
         <v>278.59899999999999</v>
@@ -52511,7 +52505,7 @@
       <c r="D11" s="2">
         <v>-2.738</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="4">
         <v>0.48099999999999998</v>
       </c>
       <c r="F11" s="4">
@@ -52534,7 +52528,7 @@
       <c r="D12" s="2">
         <v>-2.774</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="4">
         <v>0.53500000000000003</v>
       </c>
       <c r="F12" s="4">
@@ -52557,7 +52551,7 @@
       <c r="D13" s="2">
         <v>-2.8079999999999998</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="4">
         <v>0.58899999999999997</v>
       </c>
       <c r="F13" s="4">

</xml_diff>